<commit_message>
Added feature to add a product and write entry in excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/product.xlsx
+++ b/src/main/resources/excel/product.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>cream</t>
   </si>
@@ -44,12 +44,37 @@
   </si>
   <si>
     <t>parle</t>
+  </si>
+  <si>
+    <t>handwash</t>
+  </si>
+  <si>
+    <t>kenvue</t>
+  </si>
+  <si>
+    <t>lotion</t>
+  </si>
+  <si>
+    <t>jnj</t>
+  </si>
+  <si>
+    <t>skincare</t>
+  </si>
+  <si>
+    <t>kolly</t>
+  </si>
+  <si>
+    <t>wizard</t>
+  </si>
+  <si>
+    <t>harry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,6 +503,74 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>